<commit_message>
[NEAT-695] 🤓 Rename transformation to Instance Source Column (#909)
* refactor; rename transformation to instance source

* refactor: renaming

* fix: update pydantic class

* buld; changelog

* tests: updated inference

* tests: updated test

* refactor: update catalog
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav-ref.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav-ref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/docs/artifacts/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A6957C-3DCD-324F-8629-6D067616F908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB19537A-470F-442C-AB8C-C4489D90B1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="176">
   <si>
     <t>role</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>Jon,Emma,David,Alice</t>
+  </si>
+  <si>
+    <t>Instance Source</t>
   </si>
 </sst>
 </file>
@@ -745,15 +748,15 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,17 +1065,17 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0">
+    <sheetView zoomScale="208" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>171</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>173</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>83</v>
       </c>
@@ -1136,23 +1139,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="16">
         <v>45388.625104166669</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="16">
         <v>45388.625104166669</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
   </sheetData>
@@ -1180,26 +1183,26 @@
       <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1241,7 +1244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1290,7 +1293,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1364,7 +1367,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1372,7 +1375,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1399,7 +1402,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1410,7 +1413,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1456,7 +1459,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -1464,7 +1467,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -1487,41 +1490,41 @@
   </sheetPr>
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:M1"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-    </row>
-    <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1547,7 +1550,7 @@
         <v>80</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
+        <v>175</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>21</v>
@@ -1562,7 +1565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -1589,7 +1592,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1616,7 +1619,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -1643,7 +1646,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
@@ -1670,7 +1673,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1685,7 +1688,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1715,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
@@ -1739,7 +1742,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>25</v>
       </c>
@@ -1766,7 +1769,7 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
@@ -1793,7 +1796,7 @@
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -1820,7 +1823,7 @@
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1835,7 +1838,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -1862,7 +1865,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
@@ -1889,7 +1892,7 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -1916,7 +1919,7 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
@@ -1943,7 +1946,7 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1958,7 +1961,7 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>29</v>
       </c>
@@ -1985,7 +1988,7 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -2012,7 +2015,7 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -2037,7 +2040,7 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>29</v>
       </c>
@@ -2062,7 +2065,7 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2077,7 +2080,7 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
@@ -2104,7 +2107,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
@@ -2131,7 +2134,7 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -2158,7 +2161,7 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>31</v>
       </c>
@@ -2185,7 +2188,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>31</v>
       </c>
@@ -2212,7 +2215,7 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>31</v>
       </c>
@@ -2239,7 +2242,7 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>31</v>
       </c>
@@ -2266,7 +2269,7 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -2291,7 +2294,7 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>31</v>
       </c>
@@ -2316,7 +2319,7 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
@@ -2341,7 +2344,7 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -2356,7 +2359,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>41</v>
       </c>
@@ -2383,7 +2386,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
     </row>
-    <row r="36" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>41</v>
       </c>
@@ -2410,7 +2413,7 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
     </row>
-    <row r="37" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>41</v>
       </c>
@@ -2437,7 +2440,7 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
     </row>
-    <row r="38" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>41</v>
       </c>
@@ -2464,7 +2467,7 @@
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
     </row>
-    <row r="39" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -2479,7 +2482,7 @@
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
     </row>
-    <row r="40" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>51</v>
       </c>
@@ -2506,7 +2509,7 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>51</v>
       </c>
@@ -2533,7 +2536,7 @@
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>51</v>
       </c>
@@ -2558,7 +2561,7 @@
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2573,7 +2576,7 @@
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>53</v>
       </c>
@@ -2600,7 +2603,7 @@
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
     </row>
-    <row r="45" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>53</v>
       </c>
@@ -2627,7 +2630,7 @@
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
     </row>
-    <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>53</v>
       </c>
@@ -2654,7 +2657,7 @@
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
     </row>
-    <row r="47" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -2669,7 +2672,7 @@
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
     </row>
-    <row r="48" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>57</v>
       </c>
@@ -2696,7 +2699,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -2711,7 +2714,7 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>59</v>
       </c>
@@ -2738,7 +2741,7 @@
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
     </row>
-    <row r="51" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>59</v>
       </c>
@@ -2765,7 +2768,7 @@
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
     </row>
-    <row r="52" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -2780,7 +2783,7 @@
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
     </row>
-    <row r="53" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>61</v>
       </c>
@@ -2805,7 +2808,7 @@
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
     </row>
-    <row r="54" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -2820,7 +2823,7 @@
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
     </row>
-    <row r="55" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>63</v>
       </c>
@@ -2845,7 +2848,7 @@
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
     </row>
-    <row r="56" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -2860,7 +2863,7 @@
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
     </row>
-    <row r="57" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>65</v>
       </c>
@@ -2887,7 +2890,7 @@
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
     </row>
-    <row r="58" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -2902,7 +2905,7 @@
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
     </row>
-    <row r="59" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>67</v>
       </c>
@@ -2929,7 +2932,7 @@
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
     </row>
-    <row r="60" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -2944,7 +2947,7 @@
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
     </row>
-    <row r="61" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>69</v>
       </c>
@@ -2971,7 +2974,7 @@
       <c r="L61" s="6"/>
       <c r="M61" s="6"/>
     </row>
-    <row r="62" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -2986,7 +2989,7 @@
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
     </row>
-    <row r="63" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>71</v>
       </c>
@@ -3013,7 +3016,7 @@
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
     </row>
-    <row r="64" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -3028,7 +3031,7 @@
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
     </row>
-    <row r="65" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>73</v>
       </c>
@@ -3055,7 +3058,7 @@
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
     </row>
-    <row r="66" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>73</v>
       </c>

</xml_diff>